<commit_message>
Switch to PostrgreSQL database.
</commit_message>
<xml_diff>
--- a/cbc_history.xlsx
+++ b/cbc_history.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mudien/PycharmProjects/cancer_sucks/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1560739C-ABDF-9843-83AE-FC43119F5D42}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="4340" yWindow="2760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CBC_History" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -37,11 +43,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +113,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -153,7 +167,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -185,9 +199,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,6 +251,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -394,14 +444,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -421,12 +476,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>42934</v>
       </c>
       <c r="B2">
-        <v>8.050000000000001</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="C2">
         <v>12.6</v>
@@ -441,7 +496,7 @@
         <v>2978</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>42941</v>
       </c>
@@ -461,7 +516,7 @@
         <v>2521</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>42948</v>
       </c>
@@ -481,7 +536,7 @@
         <v>15334</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>42955</v>
       </c>
@@ -501,7 +556,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>42962</v>
       </c>
@@ -521,7 +576,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>42969</v>
       </c>
@@ -541,7 +596,7 @@
         <v>3823</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>42976</v>
       </c>
@@ -561,7 +616,7 @@
         <v>3742</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>42983</v>
       </c>
@@ -575,13 +630,13 @@
         <v>123</v>
       </c>
       <c r="E9">
-        <v>64.40000000000001</v>
+        <v>64.400000000000006</v>
       </c>
       <c r="F9">
         <v>8107</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>42990</v>
       </c>
@@ -601,7 +656,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>42997</v>
       </c>
@@ -609,7 +664,7 @@
         <v>6.06</v>
       </c>
       <c r="C11">
-        <v>9.199999999999999</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D11">
         <v>485</v>
@@ -621,7 +676,7 @@
         <v>1963</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>43001</v>
       </c>
@@ -629,7 +684,7 @@
         <v>4.54</v>
       </c>
       <c r="C12">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="D12">
         <v>415</v>
@@ -641,7 +696,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43004</v>
       </c>
@@ -655,13 +710,13 @@
         <v>332</v>
       </c>
       <c r="E13">
-        <v>36.3</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="F13">
         <v>1691</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>43013</v>
       </c>
@@ -675,13 +730,13 @@
         <v>243</v>
       </c>
       <c r="E14">
-        <v>38.3</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="F14">
         <v>2030</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43021</v>
       </c>
@@ -701,12 +756,12 @@
         <v>11200</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43027</v>
       </c>
       <c r="B16">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="C16">
         <v>6.8</v>
@@ -721,12 +776,12 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>43028</v>
       </c>
       <c r="B17">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="C17">
         <v>6.7</v>
@@ -741,7 +796,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43029</v>
       </c>
@@ -761,7 +816,7 @@
         <v>4143</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43038</v>
       </c>
@@ -781,12 +836,12 @@
         <v>4180</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43042</v>
       </c>
       <c r="B20">
-        <v>4.06</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="C20">
         <v>10</v>
@@ -801,7 +856,7 @@
         <v>3219</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43047</v>
       </c>
@@ -821,27 +876,27 @@
         <v>603</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>43054</v>
       </c>
       <c r="B22">
-        <v>4.14</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="C22">
-        <v>9.199999999999999</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D22">
         <v>65</v>
       </c>
       <c r="E22">
-        <v>16.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="F22">
         <v>699</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>43059</v>
       </c>
@@ -849,19 +904,19 @@
         <v>6.16</v>
       </c>
       <c r="C23">
-        <v>9.699999999999999</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D23">
         <v>357</v>
       </c>
       <c r="E23">
-        <v>38.2</v>
+        <v>38.200000000000003</v>
       </c>
       <c r="F23">
         <v>2353</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>43066</v>
       </c>
@@ -875,13 +930,13 @@
         <v>332</v>
       </c>
       <c r="E24">
-        <v>32.8</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="F24">
         <v>1751</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>43073</v>
       </c>
@@ -901,7 +956,7 @@
         <v>4115</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>43077</v>
       </c>
@@ -921,12 +976,12 @@
         <v>2950</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>43082</v>
       </c>
       <c r="B27">
-        <v>2.01</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="C27">
         <v>9.6</v>
@@ -941,7 +996,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>43086</v>
       </c>
@@ -949,7 +1004,7 @@
         <v>4.49</v>
       </c>
       <c r="C28">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="D28">
         <v>156</v>
@@ -961,7 +1016,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>43087</v>
       </c>
@@ -969,7 +1024,7 @@
         <v>4.09</v>
       </c>
       <c r="C29">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D29">
         <v>27</v>
@@ -981,7 +1036,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>43099</v>
       </c>
@@ -1001,7 +1056,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>43102</v>
       </c>

</xml_diff>